<commit_message>
added yellow in fehlende daten spreadsheet
</commit_message>
<xml_diff>
--- a/data/übersicht_datenlücken.xlsx
+++ b/data/übersicht_datenlücken.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bwedu-my.sharepoint.com/personal/alicia_pirwass_bwedu_de/Documents/Master CSE/SS21/CSEseminar_Windprognose/cse-seminar-windprognose/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="160" documentId="8_{4719C8A3-88DB-4865-9135-552785E7B723}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{1B717D26-3B63-4C62-9871-5B9570891C18}"/>
+  <xr:revisionPtr revIDLastSave="161" documentId="8_{4719C8A3-88DB-4865-9135-552785E7B723}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{84681E3D-E9D7-40B4-90EA-E6214BEB6482}"/>
   <bookViews>
-    <workbookView xWindow="50340" yWindow="2250" windowWidth="14400" windowHeight="7365" xr2:uid="{8310984F-996A-4A32-AF01-5D2AFB1DD01A}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8310984F-996A-4A32-AF01-5D2AFB1DD01A}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -466,8 +466,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BA8236A-7ED6-43B9-A1C3-220406921203}">
   <dimension ref="A1:G75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="D79" sqref="D79"/>
+    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
+      <selection activeCell="I59" sqref="I59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1281,7 +1281,7 @@
         <f>13+11</f>
         <v>24</v>
       </c>
-      <c r="D58" s="5">
+      <c r="D58" s="3">
         <v>0</v>
       </c>
       <c r="E58" s="5">

</xml_diff>